<commit_message>
on se remet dedans
</commit_message>
<xml_diff>
--- a/docs/Quetes.xlsx
+++ b/docs/Quetes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-CDA-12\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDA-08\Desktop\projet\jdr2d\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2D201A-4724-40DC-9927-E4F823EDCFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4757B6D9-9C67-446B-A198-A2B27527105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A68592E1-5DEA-40CF-958F-54ABE6EAB25D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A68592E1-5DEA-40CF-958F-54ABE6EAB25D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Quetes</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>objectifs (table annexe)</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>recuperer du houblon (Alain Chichon)</t>
@@ -571,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -628,9 +625,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -974,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D840C98-1A7E-42EE-AF78-CF32870C665E}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +984,7 @@
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1010,193 +1004,265 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>"('"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"', 0),"</f>
+        <v>('', 'Bonne brune', 'Mr Ohbar vous a demandé de faire de la bière brune', 0),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="37"/>
       <c r="E3" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="35"/>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="34"/>
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G15" si="0">"('"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"', 0),"</f>
+        <v>('', 'Bonne brune', '', 0),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="38"/>
       <c r="E4" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="36"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F4" s="35"/>
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Bonne brune', '', 0),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="22"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="37" t="s">
-        <v>34</v>
+      <c r="C5" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Coco bel œil', 'Un vampire terrorise les habitants de la ville (Iggy Pope)', 0),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="38"/>
+        <v>39</v>
+      </c>
+      <c r="D6" s="37"/>
       <c r="E6" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Coco bel œil', '', 0),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27"/>
       <c r="B7" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="39"/>
+        <v>11</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="38"/>
       <c r="E7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('avoir la batte ail', 'Coco bel œil', '', 0),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="37" t="s">
-        <v>17</v>
+      <c r="C8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Le voleur volé', 'Bernard Tappir vous demande de ramener une boubourse volée par les nains', 0),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="38"/>
+        <v>38</v>
+      </c>
+      <c r="D9" s="37"/>
       <c r="E9" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Le voleur volé', '', 0),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
       <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="39"/>
+      <c r="C10" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="38"/>
       <c r="E10" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Le voleur volé', '', 0),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Victoria secret', 'Victoria-Big-B vous demande d'aller chercher ses objets fétiches chez la reine Bours-La', 0),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="39"/>
+      <c r="C12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="38"/>
       <c r="E12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Victoria secret', '', 0),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Un carrosse dans le tunnel', 'Die Anna se sent lente, elle vous demande d'aller chercher le bipbip ', 0),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="37"/>
       <c r="E14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Un carrosse dans le tunnel', '', 0),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27"/>
       <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="39"/>
+      <c r="C15" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="38"/>
       <c r="E15" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>('', 'Un carrosse dans le tunnel', '', 0),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>

</xml_diff>